<commit_message>
cluster depending on which matrices I take
</commit_message>
<xml_diff>
--- a/TiMeS_rsfMRI_full_info.xlsx
+++ b/TiMeS_rsfMRI_full_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maylismuller/Desktop/EPFL_DOCS/Master/MA4/Project Hummel/uphummel_MA4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B319FA6-EF9A-3C44-8367-6833CF016212}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B366DDC-D092-B644-B536-45D30660511D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="available_rsfMRI" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +455,12 @@
         <bgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -468,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -513,6 +519,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,7 +743,7 @@
   <dimension ref="A1:AD1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -796,7 +805,7 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6" t="s">
         <v>8</v>
@@ -876,7 +885,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="5"/>
       <c r="F4" s="6" t="s">
         <v>8</v>
@@ -990,7 +999,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6" t="s">
         <v>17</v>
@@ -1066,7 +1075,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="5"/>
       <c r="F9" s="6" t="s">
         <v>8</v>
@@ -1180,7 +1189,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="5"/>
       <c r="F12" s="6" t="s">
         <v>8</v>
@@ -1256,7 +1265,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="5"/>
       <c r="F14" s="6" t="s">
         <v>8</v>
@@ -1294,7 +1303,7 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="5"/>
       <c r="F15" s="6" t="s">
         <v>8</v>
@@ -1370,7 +1379,7 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="5"/>
       <c r="F17" s="6" t="s">
         <v>8</v>
@@ -1408,7 +1417,7 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="5"/>
       <c r="F18" s="6" t="s">
         <v>17</v>
@@ -1482,7 +1491,7 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="5"/>
       <c r="F20" s="6" t="s">
         <v>17</v>
@@ -1520,7 +1529,7 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="8"/>
       <c r="F21" s="6" t="s">
         <v>17</v>
@@ -1558,7 +1567,7 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="5"/>
       <c r="F22" s="6" t="s">
         <v>17</v>
@@ -1710,7 +1719,7 @@
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="16"/>
       <c r="E26" s="8"/>
       <c r="F26" s="6" t="s">
         <v>8</v>
@@ -1786,7 +1795,7 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="5"/>
       <c r="F28" s="6" t="s">
         <v>8</v>
@@ -1860,7 +1869,7 @@
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="16"/>
       <c r="E30" s="8"/>
       <c r="F30" s="6" t="s">
         <v>17</v>
@@ -1936,7 +1945,7 @@
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="16"/>
       <c r="E32" s="5"/>
       <c r="F32" s="6" t="s">
         <v>8</v>
@@ -1974,7 +1983,7 @@
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="16"/>
       <c r="E33" s="8"/>
       <c r="F33" s="6" t="s">
         <v>8</v>
@@ -2012,7 +2021,7 @@
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="16"/>
       <c r="E34" s="8"/>
       <c r="F34" s="6" t="s">
         <v>17</v>
@@ -2124,7 +2133,7 @@
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="16"/>
       <c r="E37" s="5"/>
       <c r="F37" s="6" t="s">
         <v>8</v>
@@ -2238,7 +2247,7 @@
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="16"/>
       <c r="E40" s="5"/>
       <c r="F40" s="6" t="s">
         <v>8</v>
@@ -2276,7 +2285,7 @@
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="D41" s="16"/>
       <c r="E41" s="12"/>
       <c r="F41" s="6" t="s">
         <v>8</v>
@@ -2314,7 +2323,7 @@
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="16"/>
       <c r="E42" s="5"/>
       <c r="F42" s="6" t="s">
         <v>17</v>
@@ -2352,7 +2361,7 @@
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="16"/>
       <c r="E43" s="5"/>
       <c r="F43" s="6" t="s">
         <v>17</v>
@@ -2652,7 +2661,7 @@
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="5"/>
+      <c r="D51" s="16"/>
       <c r="E51" s="5"/>
       <c r="F51" s="6" t="s">
         <v>17</v>
@@ -2690,7 +2699,7 @@
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="5"/>
+      <c r="D52" s="16"/>
       <c r="E52" s="8"/>
       <c r="F52" s="6" t="s">
         <v>17</v>
@@ -2840,7 +2849,7 @@
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="5"/>
+      <c r="D56" s="16"/>
       <c r="E56" s="5"/>
       <c r="F56" s="6" t="s">
         <v>8</v>
@@ -2914,7 +2923,7 @@
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="D58" s="16"/>
       <c r="E58" s="5"/>
       <c r="F58" s="6" t="s">
         <v>8</v>
@@ -3026,7 +3035,7 @@
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="16"/>
       <c r="E61" s="8"/>
       <c r="F61" s="6" t="s">
         <v>8</v>
@@ -3214,7 +3223,7 @@
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="5"/>
+      <c r="D66" s="16"/>
       <c r="E66" s="5"/>
       <c r="F66" s="6" t="s">
         <v>8</v>
@@ -3252,7 +3261,7 @@
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+      <c r="D67" s="16"/>
       <c r="E67" s="8"/>
       <c r="F67" s="6" t="s">
         <v>17</v>
@@ -3290,7 +3299,7 @@
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+      <c r="D68" s="16"/>
       <c r="E68" s="5"/>
       <c r="F68" s="6" t="s">
         <v>8</v>
@@ -3328,7 +3337,7 @@
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+      <c r="D69" s="16"/>
       <c r="E69" s="5"/>
       <c r="F69" s="6" t="s">
         <v>8</v>
@@ -3404,7 +3413,7 @@
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="5"/>
+      <c r="D71" s="16"/>
       <c r="E71" s="8"/>
       <c r="F71" s="6" t="s">
         <v>92</v>
@@ -3518,7 +3527,7 @@
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
+      <c r="D74" s="16"/>
       <c r="E74" s="8"/>
       <c r="F74" s="6" t="s">
         <v>17</v>
@@ -3556,7 +3565,7 @@
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="D75" s="16"/>
       <c r="E75" s="5"/>
       <c r="F75" s="6" t="s">
         <v>8</v>
@@ -3594,7 +3603,7 @@
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="D76" s="16"/>
       <c r="E76" s="5"/>
       <c r="F76" s="6" t="s">
         <v>17</v>
@@ -3708,7 +3717,7 @@
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
+      <c r="D79" s="16"/>
       <c r="E79" s="8"/>
       <c r="F79" s="6" t="s">
         <v>8</v>
@@ -3784,7 +3793,7 @@
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+      <c r="D81" s="16"/>
       <c r="E81" s="8"/>
       <c r="F81" s="6" t="s">
         <v>17</v>
@@ -3822,7 +3831,7 @@
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
+      <c r="D82" s="16"/>
       <c r="E82" s="5"/>
       <c r="F82" s="6" t="s">
         <v>17</v>

</xml_diff>